<commit_message>
More figures! more results! fixed packages!
</commit_message>
<xml_diff>
--- a/results/Error_types_table.xlsx
+++ b/results/Error_types_table.xlsx
@@ -402,7 +402,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -412,7 +412,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E2">
@@ -433,7 +433,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -464,7 +464,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -474,7 +474,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E4">
@@ -495,7 +495,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -505,7 +505,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E5">
@@ -526,7 +526,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -557,7 +557,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -567,7 +567,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E7">
@@ -588,7 +588,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -619,7 +619,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E9">
@@ -650,7 +650,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -681,7 +681,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -691,7 +691,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E11">
@@ -712,7 +712,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -753,7 +753,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E13">
@@ -774,7 +774,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -784,7 +784,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E14">
@@ -805,7 +805,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -836,7 +836,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -846,7 +846,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E16">
@@ -867,7 +867,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -877,7 +877,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E17">
@@ -898,7 +898,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -929,7 +929,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -939,7 +939,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E19">
@@ -960,7 +960,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -991,7 +991,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E21">
@@ -1022,7 +1022,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E23">
@@ -1084,7 +1084,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1094,7 +1094,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E24">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1146,7 +1146,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1156,7 +1156,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E26">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1187,7 +1187,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E27">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1239,7 +1239,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E29">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1280,7 +1280,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E30">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1332,7 +1332,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E32">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1373,7 +1373,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E33">
@@ -1394,7 +1394,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1425,7 +1425,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E35">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1466,7 +1466,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E36">
@@ -1487,7 +1487,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1518,7 +1518,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E38">
@@ -1549,7 +1549,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1590,7 +1590,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E40">
@@ -1611,7 +1611,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E41">
@@ -1642,7 +1642,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E43">
@@ -1704,7 +1704,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1714,7 +1714,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E44">
@@ -1735,7 +1735,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1776,7 +1776,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E46">
@@ -1797,7 +1797,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1807,7 +1807,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E47">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1859,7 +1859,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1869,7 +1869,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E49">
@@ -1890,7 +1890,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1900,7 +1900,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E50">
@@ -1921,7 +1921,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1952,7 +1952,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1962,7 +1962,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E52">
@@ -1983,7 +1983,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E53">
@@ -2014,7 +2014,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2045,7 +2045,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2055,7 +2055,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E55">
@@ -2076,7 +2076,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2117,7 +2117,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E57">
@@ -2138,7 +2138,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2148,7 +2148,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E58">
@@ -2169,7 +2169,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2200,7 +2200,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2210,7 +2210,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E60">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2241,7 +2241,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E61">
@@ -2262,7 +2262,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2303,7 +2303,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E63">
@@ -2324,7 +2324,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2334,7 +2334,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E64">
@@ -2355,7 +2355,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2386,7 +2386,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2396,7 +2396,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E66">
@@ -2417,7 +2417,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2427,7 +2427,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E67">
@@ -2448,7 +2448,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2479,7 +2479,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E69">
@@ -2510,7 +2510,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2520,7 +2520,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E70">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2572,7 +2572,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E72">
@@ -2603,7 +2603,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E73">
@@ -2634,7 +2634,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2675,7 +2675,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E75">
@@ -2696,7 +2696,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2706,7 +2706,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E76">
@@ -2727,7 +2727,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2758,7 +2758,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E78">
@@ -2789,7 +2789,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2799,7 +2799,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E79">
@@ -2820,7 +2820,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2851,7 +2851,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2861,7 +2861,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E81">
@@ -2882,7 +2882,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2892,7 +2892,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E82">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2944,7 +2944,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E84">
@@ -2975,7 +2975,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3006,7 +3006,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3016,7 +3016,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E86">
@@ -3037,7 +3037,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3068,7 +3068,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3078,7 +3078,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E88">
@@ -3099,7 +3099,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3109,7 +3109,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E89">
@@ -3130,7 +3130,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3161,7 +3161,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3171,7 +3171,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E91">
@@ -3192,7 +3192,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3202,7 +3202,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E92">
@@ -3223,7 +3223,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3254,7 +3254,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3264,7 +3264,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E94">
@@ -3285,7 +3285,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3295,7 +3295,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E95">
@@ -3316,7 +3316,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3347,7 +3347,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E97">
@@ -3378,7 +3378,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3388,7 +3388,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E98">
@@ -3409,7 +3409,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3440,7 +3440,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3450,7 +3450,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E100">
@@ -3471,7 +3471,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3481,7 +3481,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E101">
@@ -3502,7 +3502,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3533,7 +3533,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3543,7 +3543,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E103">
@@ -3564,7 +3564,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3595,7 +3595,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3605,7 +3605,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E105">
@@ -3626,7 +3626,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3636,7 +3636,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E106">
@@ -3657,7 +3657,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3698,7 +3698,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E108">
@@ -3719,7 +3719,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E109">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3781,7 +3781,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3791,7 +3791,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E111">
@@ -3812,7 +3812,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3822,7 +3822,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E112">
@@ -3843,7 +3843,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3874,7 +3874,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3884,7 +3884,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E114">
@@ -3905,7 +3905,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3915,7 +3915,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E115">
@@ -3936,7 +3936,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -3967,7 +3967,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -3977,7 +3977,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E117">
@@ -3998,7 +3998,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -4008,7 +4008,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E118">
@@ -4029,7 +4029,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4060,7 +4060,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -4070,7 +4070,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E120">
@@ -4091,7 +4091,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -4122,7 +4122,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -4132,7 +4132,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E122">
@@ -4153,7 +4153,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -4184,7 +4184,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -4194,7 +4194,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E124">
@@ -4215,7 +4215,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -4225,7 +4225,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E125">
@@ -4246,7 +4246,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -4277,7 +4277,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -4287,7 +4287,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E127">
@@ -4308,7 +4308,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -4318,7 +4318,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E128">
@@ -4339,7 +4339,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -4370,7 +4370,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -4380,7 +4380,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E130">
@@ -4401,7 +4401,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -4411,7 +4411,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E131">
@@ -4432,7 +4432,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -4463,7 +4463,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -4473,7 +4473,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E133">
@@ -4494,7 +4494,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -4504,7 +4504,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E134">
@@ -4525,7 +4525,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -4556,7 +4556,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -4566,7 +4566,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E136">
@@ -4587,7 +4587,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -4618,7 +4618,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -4628,7 +4628,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E138">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -4680,7 +4680,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -4690,7 +4690,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E140">
@@ -4711,7 +4711,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -4721,7 +4721,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E141">
@@ -4742,7 +4742,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -4773,7 +4773,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -4783,7 +4783,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E143">
@@ -4804,7 +4804,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -4814,7 +4814,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E144">
@@ -4835,7 +4835,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -4866,7 +4866,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -4876,7 +4876,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E146">
@@ -4897,7 +4897,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -4907,7 +4907,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E147">
@@ -4928,7 +4928,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -4959,7 +4959,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -4969,7 +4969,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E149">
@@ -4990,7 +4990,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -5000,7 +5000,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E150">
@@ -5021,7 +5021,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -5052,7 +5052,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -5062,7 +5062,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E152">
@@ -5083,7 +5083,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -5114,7 +5114,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -5124,7 +5124,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E154">
@@ -5145,7 +5145,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -5155,7 +5155,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E155">
@@ -5176,7 +5176,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -5207,7 +5207,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -5217,7 +5217,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E157">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -5248,7 +5248,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Genus + species correct</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E158">
@@ -5269,7 +5269,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -5300,7 +5300,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -5310,7 +5310,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>Genus + species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E160">

</xml_diff>